<commit_message>
creation of manual docx files & adjustments to xlsx raw data file.
</commit_message>
<xml_diff>
--- a/Project 2 - Google Sheets API/Project 2 - Google Sheets API - Candy Sales Excel Raw Data.xlsx
+++ b/Project 2 - Google Sheets API/Project 2 - Google Sheets API - Candy Sales Excel Raw Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kabanda\OneDrive\Documents\Data Analysis Portfolio By Faith Kabanda\Data-Analyst-Portfolio-By-Faith-Kabanda\Project 2 - Google Sheets API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3492B8FF-55B0-4FDA-A69C-594A94E9EDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED53A70-CD41-45BC-9711-32A698C13D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:G245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>